<commit_message>
Update Tabela com Continentes
</commit_message>
<xml_diff>
--- a/TabelaTeste2.xlsx
+++ b/TabelaTeste2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Pandas Lib\Testes - 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02D6951-5139-4411-A6DA-91AA9F0A1673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585D5FD3-6E78-4C07-B7D5-2E99610B3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A591480A-62D0-784E-ADFE-D975E29332B5}"/>
   </bookViews>
@@ -17,10 +17,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'BD Final'!$H$2:$H$133</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'BD Final'!$G$2:$G$133</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'BD Final'!$D$2:$D$133</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'BD Final'!$F$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'BD Final'!$F$2:$F$133</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'BD Final'!$F$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'BD Final'!$F$2:$F$133</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'BD Final'!$D$2:$D$133</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'BD Final'!$G$2:$G$133</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'BD Final'!$E$1</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'BD Final'!$E$2:$E$133</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="287">
   <si>
     <t>Brazil</t>
   </si>
@@ -851,24 +851,12 @@
     <t>PIB</t>
   </si>
   <si>
-    <t>Expectativa de Vida (em anos)</t>
-  </si>
-  <si>
-    <t>Acesso Internet (pessoas)</t>
-  </si>
-  <si>
     <t>Índice de Felicidade (0-10)</t>
   </si>
   <si>
     <t>População</t>
   </si>
   <si>
-    <t>média</t>
-  </si>
-  <si>
-    <t>desv pad</t>
-  </si>
-  <si>
     <t>IF PADRONIZADA</t>
   </si>
   <si>
@@ -888,6 +876,36 @@
   </si>
   <si>
     <t>ALTA</t>
+  </si>
+  <si>
+    <t>Continente</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>África</t>
+  </si>
+  <si>
+    <t>América do Sul</t>
+  </si>
+  <si>
+    <t>Ásia</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>América do Norte</t>
+  </si>
+  <si>
+    <t>América Central</t>
+  </si>
+  <si>
+    <t>Expectativa de Vida</t>
+  </si>
+  <si>
+    <t>Acesso Internet</t>
   </si>
 </sst>
 </file>
@@ -895,8 +913,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -940,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -954,11 +972,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5790,7 +5811,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5851,7 +5872,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5889,8 +5910,8 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{60E10D99-FFF3-4C5B-8D50-1EA0B3DDECBB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
-              <cx:v>Expectativa de Vida (em anos)</cx:v>
+              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:v>Expectativa de Vida</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -5985,7 +6006,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -10197,7 +10218,7 @@
   <dimension ref="A1:M137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10210,7 +10231,7 @@
     <col min="6" max="6" width="26.375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="1"/>
+    <col min="9" max="9" width="22.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.25" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="81.125" style="1" bestFit="1" customWidth="1"/>
@@ -10228,28 +10249,31 @@
         <v>266</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>267</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>274</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -10277,19 +10301,18 @@
       <c r="H2" s="2">
         <v>4.8826999999999998</v>
       </c>
-      <c r="I2" s="1" t="str">
-        <f>IF(F2&lt;40,"ESTEVÃO","DEPAY")</f>
-        <v>DEPAY</v>
+      <c r="I2" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K2" s="1">
         <f>(H2-$H$136)/$H$137</f>
         <v>-0.6067752030614969</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -10317,15 +10340,14 @@
       <c r="H3" s="2">
         <v>5.0050999999999997</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I66" si="0">IF(F3&lt;40,"ESTEVÃO","DEPAY")</f>
-        <v>DEPAY</v>
+      <c r="I3" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K66" si="1">(H3-$H$136)/$H$137</f>
+        <f t="shared" ref="K3:K66" si="0">(H3-$H$136)/$H$137</f>
         <v>-0.4955616026909499</v>
       </c>
     </row>
@@ -10354,15 +10376,14 @@
       <c r="H4" s="2">
         <v>5.9747000000000003</v>
       </c>
-      <c r="I4" s="1" t="str">
+      <c r="I4" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K4" s="1">
-        <f t="shared" si="1"/>
         <v>0.38542456495024796</v>
       </c>
     </row>
@@ -10391,15 +10412,14 @@
       <c r="H5" s="2">
         <v>4.6768000000000001</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="I5" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="1"/>
         <v>-0.79385755858678808</v>
       </c>
     </row>
@@ -10428,15 +10448,14 @@
       <c r="H6" s="2">
         <v>7.2228000000000003</v>
       </c>
-      <c r="I6" s="1" t="str">
+      <c r="I6" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="1"/>
         <v>1.5194580177482866</v>
       </c>
     </row>
@@ -10465,15 +10484,14 @@
       <c r="H7" s="2">
         <v>7.2942</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="I7" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="1"/>
         <v>1.5843326179644388</v>
       </c>
     </row>
@@ -10502,15 +10520,14 @@
       <c r="H8" s="2">
         <v>5.1647999999999996</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="I8" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="1"/>
         <v>-0.35045692965846315</v>
       </c>
     </row>
@@ -10539,15 +10556,14 @@
       <c r="H9" s="2">
         <v>6.2272999999999996</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="I9" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="1"/>
         <v>0.6149389068914255</v>
       </c>
     </row>
@@ -10576,15 +10592,14 @@
       <c r="H10" s="2">
         <v>4.8327999999999998</v>
       </c>
-      <c r="I10" s="1" t="str">
+      <c r="I10" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="1"/>
         <v>-0.6521147345851106</v>
       </c>
     </row>
@@ -10613,15 +10628,14 @@
       <c r="H11" s="2">
         <v>5.5399000000000003</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="I11" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="1"/>
         <v>-9.6381265621206646E-3</v>
       </c>
     </row>
@@ -10650,15 +10664,14 @@
       <c r="H12" s="2">
         <v>6.8635000000000002</v>
       </c>
-      <c r="I12" s="1" t="str">
+      <c r="I12" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="1"/>
         <v>1.1929952186213453</v>
       </c>
     </row>
@@ -10687,15 +10700,14 @@
       <c r="H13" s="2">
         <v>5.2160000000000002</v>
       </c>
-      <c r="I13" s="1" t="str">
+      <c r="I13" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="1"/>
         <v>-0.30393620793483506</v>
       </c>
     </row>
@@ -10724,15 +10736,14 @@
       <c r="H14" s="2">
         <v>5.7474999999999996</v>
       </c>
-      <c r="I14" s="1" t="str">
+      <c r="I14" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K14" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K14" s="1">
-        <f t="shared" si="1"/>
         <v>0.17898886230164993</v>
       </c>
     </row>
@@ -10761,15 +10772,14 @@
       <c r="H15" s="2">
         <v>5.6741000000000001</v>
       </c>
-      <c r="I15" s="1" t="str">
+      <c r="I15" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K15" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="1"/>
         <v>0.11229704639316869</v>
       </c>
     </row>
@@ -10798,19 +10808,18 @@
       <c r="H16" s="2">
         <v>3.4788999999999999</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="I16" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="1"/>
         <v>-1.8822788975073639</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -10838,15 +10847,14 @@
       <c r="H17" s="2">
         <v>6.3756000000000004</v>
       </c>
-      <c r="I17" s="1" t="str">
+      <c r="I17" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K17" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="1"/>
         <v>0.74968545047763657</v>
       </c>
       <c r="L17" s="1">
@@ -10879,15 +10887,14 @@
       <c r="H18" s="2">
         <v>5.1014999999999997</v>
       </c>
-      <c r="I18" s="1" t="str">
+      <c r="I18" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K18" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="1"/>
         <v>-0.40797180632068231</v>
       </c>
     </row>
@@ -10916,15 +10923,14 @@
       <c r="H19" s="2">
         <v>4.7686999999999999</v>
       </c>
-      <c r="I19" s="1" t="str">
+      <c r="I19" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K19" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K19" s="1">
-        <f t="shared" si="1"/>
         <v>-0.71035649752426133</v>
       </c>
       <c r="L19" s="6">
@@ -10957,15 +10963,14 @@
       <c r="H20" s="2">
         <v>3.7753000000000001</v>
       </c>
-      <c r="I20" s="1" t="str">
+      <c r="I20" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K20" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K20" s="1">
-        <f t="shared" si="1"/>
         <v>-1.6129675319041759</v>
       </c>
     </row>
@@ -10994,15 +10999,14 @@
       <c r="H21" s="2">
         <v>5.0849000000000002</v>
       </c>
-      <c r="I21" s="1" t="str">
+      <c r="I21" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K21" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K21" s="1">
-        <f t="shared" si="1"/>
         <v>-0.42305469656701422</v>
       </c>
     </row>
@@ -11031,15 +11035,14 @@
       <c r="H22" s="2">
         <v>7.2321</v>
       </c>
-      <c r="I22" s="1" t="str">
+      <c r="I22" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K22" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" si="1"/>
         <v>1.5279080707176171</v>
       </c>
     </row>
@@ -11068,15 +11071,14 @@
       <c r="H23" s="2">
         <v>3.4759000000000002</v>
       </c>
-      <c r="I23" s="1" t="str">
+      <c r="I23" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K23" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K23" s="1">
-        <f t="shared" si="1"/>
         <v>-1.8850047210458574</v>
       </c>
     </row>
@@ -11105,15 +11107,14 @@
       <c r="H24" s="2">
         <v>4.4226999999999999</v>
       </c>
-      <c r="I24" s="1" t="str">
+      <c r="I24" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K24" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K24" s="1">
-        <f t="shared" si="1"/>
         <v>-1.0247348122972133</v>
       </c>
     </row>
@@ -11142,15 +11143,14 @@
       <c r="H25" s="2">
         <v>6.2285000000000004</v>
       </c>
-      <c r="I25" s="1" t="str">
+      <c r="I25" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K25" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K25" s="1">
-        <f t="shared" si="1"/>
         <v>0.61602923630682371</v>
       </c>
     </row>
@@ -11179,15 +11179,14 @@
       <c r="H26" s="2">
         <v>5.1238999999999999</v>
       </c>
-      <c r="I26" s="1" t="str">
+      <c r="I26" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K26" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K26" s="1">
-        <f t="shared" si="1"/>
         <v>-0.38761899056659505</v>
       </c>
     </row>
@@ -11216,15 +11215,14 @@
       <c r="H27" s="2">
         <v>6.1634000000000002</v>
       </c>
-      <c r="I27" s="1" t="str">
+      <c r="I27" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K27" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K27" s="1">
-        <f t="shared" si="1"/>
         <v>0.55687886552150812</v>
       </c>
     </row>
@@ -11253,15 +11251,14 @@
       <c r="H28" s="2">
         <v>7.1214000000000004</v>
       </c>
-      <c r="I28" s="1" t="str">
+      <c r="I28" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K28" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" si="1"/>
         <v>1.4273251821471962</v>
       </c>
     </row>
@@ -11290,15 +11287,14 @@
       <c r="H29" s="2">
         <v>5.2332999999999998</v>
       </c>
-      <c r="I29" s="1" t="str">
+      <c r="I29" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K29" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" si="1"/>
         <v>-0.28821729219618775</v>
       </c>
     </row>
@@ -11327,15 +11323,14 @@
       <c r="H30" s="2">
         <v>5.5046999999999997</v>
       </c>
-      <c r="I30" s="1" t="str">
+      <c r="I30" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K30" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K30" s="1">
-        <f t="shared" si="1"/>
         <v>-4.1621122747115137E-2</v>
       </c>
     </row>
@@ -11364,15 +11359,14 @@
       <c r="H31" s="2">
         <v>6.1589999999999998</v>
       </c>
-      <c r="I31" s="1" t="str">
+      <c r="I31" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K31" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="1"/>
         <v>0.5528809909983835</v>
       </c>
     </row>
@@ -11401,15 +11395,14 @@
       <c r="H32" s="2">
         <v>6.9108999999999998</v>
       </c>
-      <c r="I32" s="1" t="str">
+      <c r="I32" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K32" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K32" s="1">
-        <f t="shared" si="1"/>
         <v>1.2360632305295471</v>
       </c>
     </row>
@@ -11438,15 +11431,14 @@
       <c r="H33" s="2">
         <v>4.3109999999999999</v>
       </c>
-      <c r="I33" s="1" t="str">
+      <c r="I33" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K33" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K33" s="1">
-        <f t="shared" si="1"/>
         <v>-1.1262263087137991</v>
       </c>
     </row>
@@ -11475,15 +11467,14 @@
       <c r="H34" s="2">
         <v>7.6456</v>
       </c>
-      <c r="I34" s="1" t="str">
+      <c r="I34" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K34" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K34" s="1">
-        <f t="shared" si="1"/>
         <v>1.9036174151066796</v>
       </c>
     </row>
@@ -11512,15 +11503,14 @@
       <c r="H35" s="2">
         <v>5.6891999999999996</v>
       </c>
-      <c r="I35" s="1" t="str">
+      <c r="I35" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K35" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K35" s="1">
-        <f t="shared" si="1"/>
         <v>0.12601702487025365</v>
       </c>
     </row>
@@ -11549,15 +11539,14 @@
       <c r="H36" s="2">
         <v>5.9252000000000002</v>
       </c>
-      <c r="I36" s="1" t="str">
+      <c r="I36" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K36" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K36" s="1">
-        <f t="shared" si="1"/>
         <v>0.34044847656510013</v>
       </c>
     </row>
@@ -11586,15 +11575,14 @@
       <c r="H37" s="2">
         <v>4.1513999999999998</v>
       </c>
-      <c r="I37" s="1" t="str">
+      <c r="I37" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K37" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="1"/>
         <v>-1.2712401209616697</v>
       </c>
     </row>
@@ -11623,15 +11611,14 @@
       <c r="H38" s="2">
         <v>6.3483000000000001</v>
       </c>
-      <c r="I38" s="1" t="str">
+      <c r="I38" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K38" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K38" s="1">
-        <f t="shared" si="1"/>
         <v>0.72488045627734266</v>
       </c>
     </row>
@@ -11660,15 +11647,14 @@
       <c r="H39" s="2">
         <v>6.0217999999999998</v>
       </c>
-      <c r="I39" s="1" t="str">
+      <c r="I39" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K39" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K39" s="1">
-        <f t="shared" si="1"/>
         <v>0.42821999450460019</v>
       </c>
     </row>
@@ -11697,15 +11683,14 @@
       <c r="H40" s="2">
         <v>4.1862000000000004</v>
       </c>
-      <c r="I40" s="1" t="str">
+      <c r="I40" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K40" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K40" s="1">
-        <f t="shared" si="1"/>
         <v>-1.2396205679151411</v>
       </c>
     </row>
@@ -11734,15 +11719,14 @@
       <c r="H41" s="2">
         <v>7.8087</v>
       </c>
-      <c r="I41" s="1" t="str">
+      <c r="I41" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K41" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K41" s="1">
-        <f t="shared" si="1"/>
         <v>2.0518113548161261</v>
       </c>
     </row>
@@ -11771,15 +11755,14 @@
       <c r="H42" s="2">
         <v>6.6638000000000002</v>
       </c>
-      <c r="I42" s="1" t="str">
+      <c r="I42" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K42" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K42" s="1">
-        <f t="shared" si="1"/>
         <v>1.0115462317422743</v>
       </c>
     </row>
@@ -11808,15 +11791,14 @@
       <c r="H43" s="2">
         <v>4.8292999999999999</v>
       </c>
-      <c r="I43" s="1" t="str">
+      <c r="I43" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K43" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K43" s="1">
-        <f t="shared" si="1"/>
         <v>-0.65529486204668652</v>
       </c>
     </row>
@@ -11845,15 +11827,14 @@
       <c r="H44" s="2">
         <v>4.7506000000000004</v>
       </c>
-      <c r="I44" s="1" t="str">
+      <c r="I44" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K44" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K44" s="1">
-        <f t="shared" si="1"/>
         <v>-0.72680229953984021</v>
       </c>
     </row>
@@ -11882,15 +11863,14 @@
       <c r="H45" s="2">
         <v>4.6726000000000001</v>
       </c>
-      <c r="I45" s="1" t="str">
+      <c r="I45" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K45" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K45" s="1">
-        <f t="shared" si="1"/>
         <v>-0.79767371154067934</v>
       </c>
     </row>
@@ -11919,15 +11899,14 @@
       <c r="H46" s="2">
         <v>7.0758000000000001</v>
       </c>
-      <c r="I46" s="1" t="str">
+      <c r="I46" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K46" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K46" s="1">
-        <f t="shared" si="1"/>
         <v>1.3858926643620899</v>
       </c>
     </row>
@@ -11956,15 +11935,14 @@
       <c r="H47" s="2">
         <v>5.1479999999999997</v>
       </c>
-      <c r="I47" s="1" t="str">
+      <c r="I47" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K47" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K47" s="1">
-        <f t="shared" si="1"/>
         <v>-0.36572154147402836</v>
       </c>
     </row>
@@ -11993,15 +11971,14 @@
       <c r="H48" s="2">
         <v>5.5149999999999997</v>
       </c>
-      <c r="I48" s="1" t="str">
+      <c r="I48" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K48" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K48" s="1">
-        <f t="shared" si="1"/>
         <v>-3.2262461931619767E-2</v>
       </c>
     </row>
@@ -12030,15 +12007,14 @@
       <c r="H49" s="2">
         <v>6.3989000000000003</v>
       </c>
-      <c r="I49" s="1" t="str">
+      <c r="I49" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K49" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K49" s="1">
-        <f t="shared" si="1"/>
         <v>0.77085601329327169</v>
       </c>
     </row>
@@ -12067,15 +12043,14 @@
       <c r="H50" s="2">
         <v>4.9493</v>
       </c>
-      <c r="I50" s="1" t="str">
+      <c r="I50" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K50" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K50" s="1">
-        <f t="shared" si="1"/>
         <v>-0.54626192050693434</v>
       </c>
     </row>
@@ -12104,15 +12079,14 @@
       <c r="H51" s="2">
         <v>3.7208000000000001</v>
       </c>
-      <c r="I51" s="1" t="str">
+      <c r="I51" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K51" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K51" s="1">
-        <f t="shared" si="1"/>
         <v>-1.6624866595201466</v>
       </c>
     </row>
@@ -12141,15 +12115,14 @@
       <c r="H52" s="2">
         <v>5.9531999999999998</v>
       </c>
-      <c r="I52" s="1" t="str">
+      <c r="I52" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K52" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K52" s="1">
-        <f t="shared" si="1"/>
         <v>0.36588949625770856</v>
       </c>
     </row>
@@ -12178,15 +12151,14 @@
       <c r="H53" s="2">
         <v>5.5103999999999997</v>
       </c>
-      <c r="I53" s="1" t="str">
+      <c r="I53" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K53" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="1"/>
         <v>-3.6442058023976875E-2</v>
       </c>
     </row>
@@ -12215,15 +12187,14 @@
       <c r="H54" s="2">
         <v>6.0004</v>
       </c>
-      <c r="I54" s="1" t="str">
+      <c r="I54" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K54" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K54" s="1">
-        <f t="shared" si="1"/>
         <v>0.40877578659667785</v>
       </c>
     </row>
@@ -12252,15 +12223,14 @@
       <c r="H55" s="2">
         <v>7.5045000000000002</v>
       </c>
-      <c r="I55" s="1" t="str">
+      <c r="I55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K55" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="1"/>
         <v>1.7754128480128546</v>
       </c>
     </row>
@@ -12289,15 +12259,14 @@
       <c r="H56" s="2">
         <v>3.5733000000000001</v>
       </c>
-      <c r="I56" s="1" t="str">
+      <c r="I56" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K56" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K56" s="1">
-        <f t="shared" si="1"/>
         <v>-1.7965063168294253</v>
       </c>
     </row>
@@ -12326,15 +12295,14 @@
       <c r="H57" s="2">
         <v>5.2855999999999996</v>
       </c>
-      <c r="I57" s="1" t="str">
+      <c r="I57" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K57" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K57" s="1">
-        <f t="shared" si="1"/>
         <v>-0.24069710184177931</v>
       </c>
     </row>
@@ -12363,15 +12331,14 @@
       <c r="H58" s="2">
         <v>4.6723999999999997</v>
       </c>
-      <c r="I58" s="1" t="str">
+      <c r="I58" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K58" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K58" s="1">
-        <f t="shared" si="1"/>
         <v>-0.79785543310991269</v>
       </c>
     </row>
@@ -12400,15 +12367,14 @@
       <c r="H59" s="2">
         <v>4.7847999999999997</v>
       </c>
-      <c r="I59" s="1" t="str">
+      <c r="I59" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K59" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K59" s="1">
-        <f t="shared" si="1"/>
         <v>-0.69572791120101141</v>
       </c>
     </row>
@@ -12437,15 +12403,14 @@
       <c r="H60" s="2">
         <v>7.0937000000000001</v>
       </c>
-      <c r="I60" s="1" t="str">
+      <c r="I60" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K60" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K60" s="1">
-        <f t="shared" si="1"/>
         <v>1.4021567448084364</v>
       </c>
     </row>
@@ -12474,15 +12439,14 @@
       <c r="H61" s="2">
         <v>7.1285999999999996</v>
       </c>
-      <c r="I61" s="1" t="str">
+      <c r="I61" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K61" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K61" s="1">
-        <f t="shared" si="1"/>
         <v>1.4338671586395806</v>
       </c>
     </row>
@@ -12511,15 +12475,14 @@
       <c r="H62" s="2">
         <v>6.3874000000000004</v>
       </c>
-      <c r="I62" s="1" t="str">
+      <c r="I62" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K62" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K62" s="1">
-        <f t="shared" si="1"/>
         <v>0.76040702306237895</v>
       </c>
     </row>
@@ -12548,15 +12511,14 @@
       <c r="H63" s="2">
         <v>5.8708</v>
       </c>
-      <c r="I63" s="1" t="str">
+      <c r="I63" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K63" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K63" s="1">
-        <f t="shared" si="1"/>
         <v>0.29102020973374559</v>
       </c>
     </row>
@@ -12585,15 +12547,14 @@
       <c r="H64" s="2">
         <v>6.0579000000000001</v>
       </c>
-      <c r="I64" s="1" t="str">
+      <c r="I64" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K64" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K64" s="1">
-        <f t="shared" si="1"/>
         <v>0.4610207377511425</v>
       </c>
     </row>
@@ -12622,15 +12583,14 @@
       <c r="H65" s="2">
         <v>4.5830000000000002</v>
       </c>
-      <c r="I65" s="1" t="str">
+      <c r="I65" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K65" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K65" s="1">
-        <f t="shared" si="1"/>
         <v>-0.8790849745570275</v>
       </c>
     </row>
@@ -12659,15 +12619,14 @@
       <c r="H66" s="2">
         <v>6.1021000000000001</v>
       </c>
-      <c r="I66" s="1" t="str">
+      <c r="I66" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K66" s="1">
         <f t="shared" si="0"/>
-        <v>DEPAY</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K66" s="1">
-        <f t="shared" si="1"/>
         <v>0.50118120455161785</v>
       </c>
     </row>
@@ -12696,15 +12655,14 @@
       <c r="H67" s="2">
         <v>5.5415000000000001</v>
       </c>
-      <c r="I67" s="1" t="str">
-        <f t="shared" ref="I67:I130" si="2">IF(F67&lt;40,"ESTEVÃO","DEPAY")</f>
-        <v>DEPAY</v>
+      <c r="I67" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" ref="K67:K130" si="3">(H67-$H$136)/$H$137</f>
+        <f t="shared" ref="K67:K130" si="1">(H67-$H$136)/$H$137</f>
         <v>-8.1843540082574637E-3</v>
       </c>
     </row>
@@ -12733,15 +12691,14 @@
       <c r="H68" s="2">
         <v>4.8886000000000003</v>
       </c>
-      <c r="I68" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I68" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.60141441676912533</v>
       </c>
     </row>
@@ -12770,15 +12727,14 @@
       <c r="H69" s="2">
         <v>5.95</v>
       </c>
-      <c r="I69" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I69" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.36298195114998216</v>
       </c>
     </row>
@@ -12807,15 +12763,14 @@
       <c r="H70" s="2">
         <v>4.7714999999999996</v>
       </c>
-      <c r="I70" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I70" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.70781239555500075</v>
       </c>
     </row>
@@ -12844,15 +12799,14 @@
       <c r="H71" s="2">
         <v>3.6528</v>
       </c>
-      <c r="I71" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I71" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.7242719930593395</v>
       </c>
     </row>
@@ -12881,15 +12835,14 @@
       <c r="H72" s="2">
         <v>4.5579000000000001</v>
       </c>
-      <c r="I72" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I72" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.90189103149575911</v>
       </c>
     </row>
@@ -12918,15 +12871,14 @@
       <c r="H73" s="2">
         <v>6.2154999999999996</v>
       </c>
-      <c r="I73" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I73" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.60421733430668323</v>
       </c>
     </row>
@@ -12955,15 +12907,14 @@
       <c r="H74" s="2">
         <v>7.2374999999999998</v>
       </c>
-      <c r="I74" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I74" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.5328145530869057</v>
       </c>
     </row>
@@ -12992,15 +12943,14 @@
       <c r="H75" s="2">
         <v>3.5379999999999998</v>
       </c>
-      <c r="I75" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I75" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.8285801737990359</v>
       </c>
     </row>
@@ -13029,15 +12979,14 @@
       <c r="H76" s="2">
         <v>5.3842999999999996</v>
       </c>
-      <c r="I76" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I76" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.15101750742533315</v>
       </c>
     </row>
@@ -13066,15 +13015,14 @@
       <c r="H77" s="2">
         <v>5.1976000000000004</v>
       </c>
-      <c r="I77" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I77" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.32065459230426346</v>
       </c>
     </row>
@@ -13103,15 +13051,14 @@
       <c r="H78" s="2">
         <v>4.7293000000000003</v>
       </c>
-      <c r="I78" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I78" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.74615564666314627</v>
       </c>
     </row>
@@ -13140,15 +13087,14 @@
       <c r="H79" s="2">
         <v>6.7728000000000002</v>
       </c>
-      <c r="I79" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I79" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.1105844869742159</v>
       </c>
     </row>
@@ -13177,15 +13123,14 @@
       <c r="H80" s="2">
         <v>4.3746</v>
       </c>
-      <c r="I80" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I80" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.0684388496977306</v>
       </c>
     </row>
@@ -13214,15 +13159,14 @@
       <c r="H81" s="2">
         <v>6.1013000000000002</v>
       </c>
-      <c r="I81" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I81" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.50045431827468634</v>
       </c>
     </row>
@@ -13251,15 +13195,14 @@
       <c r="H82" s="2">
         <v>6.4649999999999999</v>
       </c>
-      <c r="I82" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I82" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.83091499192475149</v>
       </c>
     </row>
@@ -13288,15 +13231,14 @@
       <c r="H83" s="2">
         <v>5.4561999999999999</v>
       </c>
-      <c r="I83" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I83" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-8.5688603286098078E-2</v>
       </c>
     </row>
@@ -13325,15 +13267,14 @@
       <c r="H84" s="2">
         <v>5.5461</v>
       </c>
-      <c r="I84" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I84" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-4.004757915900355E-3</v>
       </c>
     </row>
@@ -13362,15 +13303,14 @@
       <c r="H85" s="2">
         <v>5.0948000000000002</v>
       </c>
-      <c r="I85" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I85" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.41405947888998468</v>
       </c>
     </row>
@@ -13399,15 +13339,14 @@
       <c r="H86" s="2">
         <v>4.6235999999999997</v>
       </c>
-      <c r="I86" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I86" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.84219549600274513</v>
       </c>
     </row>
@@ -13436,15 +13375,14 @@
       <c r="H87" s="2">
         <v>4.3079999999999998</v>
       </c>
-      <c r="I87" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I87" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.1289521322522931</v>
       </c>
     </row>
@@ -13473,15 +13411,14 @@
       <c r="H88" s="2">
         <v>4.5711000000000004</v>
       </c>
-      <c r="I88" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I88" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.88989740792638605</v>
       </c>
     </row>
@@ -13510,15 +13447,14 @@
       <c r="H89" s="2">
         <v>5.1372</v>
       </c>
-      <c r="I89" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I89" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.37553450621260576</v>
       </c>
     </row>
@@ -13547,15 +13483,14 @@
       <c r="H90" s="2">
         <v>7.4489000000000001</v>
       </c>
-      <c r="I90" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I90" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.7248942517661026</v>
       </c>
     </row>
@@ -13584,15 +13519,14 @@
       <c r="H91" s="2">
         <v>7.2995999999999999</v>
       </c>
-      <c r="I91" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I91" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.5892391003337276</v>
       </c>
     </row>
@@ -13621,15 +13555,14 @@
       <c r="H92" s="2">
         <v>6.1371000000000002</v>
       </c>
-      <c r="I92" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I92" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.53298247916737906</v>
       </c>
     </row>
@@ -13658,15 +13591,14 @@
       <c r="H93" s="2">
         <v>4.7241</v>
       </c>
-      <c r="I93" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I93" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.7508804074632025</v>
       </c>
     </row>
@@ -13695,15 +13627,14 @@
       <c r="H94" s="2">
         <v>5.1597999999999997</v>
       </c>
-      <c r="I94" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I94" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.35499996888928603</v>
       </c>
     </row>
@@ -13732,15 +13663,14 @@
       <c r="H95" s="2">
         <v>7.4880000000000004</v>
       </c>
-      <c r="I95" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I95" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.760420818551139</v>
       </c>
     </row>
@@ -13769,15 +13699,14 @@
       <c r="H96" s="2">
         <v>5.6932999999999998</v>
       </c>
-      <c r="I96" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I96" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K96" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.12974231703952871</v>
       </c>
     </row>
@@ -13806,15 +13735,14 @@
       <c r="H97" s="2">
         <v>4.5528000000000004</v>
       </c>
-      <c r="I97" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I97" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K97" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.90652493151119828</v>
       </c>
     </row>
@@ -13843,15 +13771,14 @@
       <c r="H98" s="2">
         <v>6.3048000000000002</v>
       </c>
-      <c r="I98" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I98" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K98" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.68535601496918264</v>
       </c>
     </row>
@@ -13880,15 +13807,14 @@
       <c r="H99" s="2">
         <v>5.6920999999999999</v>
       </c>
-      <c r="I99" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I99" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K99" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.12865198762413133</v>
       </c>
     </row>
@@ -13917,15 +13843,14 @@
       <c r="H100" s="2">
         <v>5.7968000000000002</v>
       </c>
-      <c r="I100" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I100" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K100" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.22378322911756526</v>
       </c>
     </row>
@@ -13954,15 +13879,14 @@
       <c r="H101" s="2">
         <v>6.0060000000000002</v>
       </c>
-      <c r="I101" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I101" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K101" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.41386399053519984</v>
       </c>
     </row>
@@ -13991,15 +13915,14 @@
       <c r="H102" s="2">
         <v>6.1863000000000001</v>
       </c>
-      <c r="I102" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I102" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K102" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.57768598519867731</v>
       </c>
     </row>
@@ -14028,15 +13951,14 @@
       <c r="H103" s="2">
         <v>5.9108999999999998</v>
       </c>
-      <c r="I103" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I103" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K103" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.32745538436494592</v>
       </c>
     </row>
@@ -14065,15 +13987,14 @@
       <c r="H104" s="2">
         <v>6.1237000000000004</v>
       </c>
-      <c r="I104" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I104" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K104" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.52080713402877354</v>
       </c>
     </row>
@@ -14102,15 +14023,14 @@
       <c r="H105" s="2">
         <v>5.5460000000000003</v>
       </c>
-      <c r="I105" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I105" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K105" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-4.0956187005166036E-3</v>
       </c>
     </row>
@@ -14139,15 +14059,14 @@
       <c r="H106" s="2">
         <v>3.3123</v>
       </c>
-      <c r="I106" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I106" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K106" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-2.0336529646783861</v>
       </c>
     </row>
@@ -14176,15 +14095,14 @@
       <c r="H107" s="2">
         <v>6.4065000000000003</v>
       </c>
-      <c r="I107" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I107" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K107" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.7777614329241227</v>
       </c>
     </row>
@@ -14213,15 +14131,14 @@
       <c r="H108" s="2">
         <v>4.9808000000000003</v>
       </c>
-      <c r="I108" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I108" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K108" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.51764077335274905</v>
       </c>
     </row>
@@ -14250,15 +14167,14 @@
       <c r="H109" s="2">
         <v>5.7782</v>
       </c>
-      <c r="I109" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I109" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K109" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.20688312317890353</v>
       </c>
     </row>
@@ -14287,15 +14203,14 @@
       <c r="H110" s="2">
         <v>3.9264000000000001</v>
       </c>
-      <c r="I110" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I110" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K110" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.4756768863487046</v>
       </c>
     </row>
@@ -14324,15 +14239,14 @@
       <c r="H111" s="2">
         <v>6.3771000000000004</v>
       </c>
-      <c r="I111" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I111" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K111" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.75104836224688354</v>
       </c>
     </row>
@@ -14361,15 +14275,14 @@
       <c r="H112" s="2">
         <v>6.2805999999999997</v>
       </c>
-      <c r="I112" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I112" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K112" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.66336770509199894</v>
       </c>
     </row>
@@ -14398,15 +14311,14 @@
       <c r="H113" s="2">
         <v>6.3634000000000004</v>
       </c>
-      <c r="I113" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I113" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K113" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.73860043475442849</v>
       </c>
     </row>
@@ -14435,15 +14347,14 @@
       <c r="H114" s="2">
         <v>4.8140999999999998</v>
       </c>
-      <c r="I114" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I114" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K114" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.66910570130838853</v>
       </c>
     </row>
@@ -14472,15 +14383,14 @@
       <c r="H115" s="2">
         <v>5.8723999999999998</v>
       </c>
-      <c r="I115" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I115" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K115" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.29247398228760879</v>
       </c>
     </row>
@@ -14509,15 +14419,14 @@
       <c r="H116" s="2">
         <v>6.4009</v>
       </c>
-      <c r="I116" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I116" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K116" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.77267322898560065</v>
       </c>
     </row>
@@ -14546,15 +14455,14 @@
       <c r="H117" s="2">
         <v>4.327</v>
       </c>
-      <c r="I117" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I117" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K117" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.1116885831751657</v>
       </c>
     </row>
@@ -14583,15 +14491,14 @@
       <c r="H118" s="2">
         <v>7.3535000000000004</v>
       </c>
-      <c r="I118" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I118" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K118" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.638213063242</v>
       </c>
     </row>
@@ -14620,15 +14527,14 @@
       <c r="H119" s="2">
         <v>7.5598999999999998</v>
       </c>
-      <c r="I119" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I119" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K119" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8257497226903732</v>
       </c>
     </row>
@@ -14657,15 +14563,14 @@
       <c r="H120" s="2">
         <v>3.4762</v>
       </c>
-      <c r="I120" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I120" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K120" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.8847321386920082</v>
       </c>
     </row>
@@ -14694,15 +14599,14 @@
       <c r="H121" s="2">
         <v>5.9988000000000001</v>
       </c>
-      <c r="I121" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I121" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K121" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.40732201404281465</v>
       </c>
     </row>
@@ -14731,15 +14635,14 @@
       <c r="H122" s="2">
         <v>4.1871999999999998</v>
       </c>
-      <c r="I122" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I122" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K122" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.2387119600689769</v>
       </c>
     </row>
@@ -14768,15 +14671,14 @@
       <c r="H123" s="2">
         <v>4.3921999999999999</v>
       </c>
-      <c r="I123" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I123" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K123" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.0524473516052337</v>
       </c>
     </row>
@@ -14805,15 +14707,14 @@
       <c r="H124" s="2">
         <v>5.1318000000000001</v>
       </c>
-      <c r="I124" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I124" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K124" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.38044098858189451</v>
       </c>
     </row>
@@ -14842,15 +14743,14 @@
       <c r="H125" s="2">
         <v>4.4320000000000004</v>
       </c>
-      <c r="I125" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I125" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K125" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1.0162847593278821</v>
       </c>
     </row>
@@ -14879,15 +14779,14 @@
       <c r="H126" s="2">
         <v>4.5606999999999998</v>
       </c>
-      <c r="I126" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I126" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K126" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-0.89934692952649853</v>
       </c>
     </row>
@@ -14916,15 +14815,14 @@
       <c r="H127" s="2">
         <v>6.7907999999999999</v>
       </c>
-      <c r="I127" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I127" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K127" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.1269394282051786</v>
       </c>
     </row>
@@ -14953,15 +14851,14 @@
       <c r="H128" s="2">
         <v>7.1645000000000003</v>
       </c>
-      <c r="I128" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I128" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K128" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.4664861803168903</v>
       </c>
     </row>
@@ -14990,15 +14887,14 @@
       <c r="H129" s="2">
         <v>6.9396000000000004</v>
       </c>
-      <c r="I129" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I129" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K129" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.2621402757144717</v>
       </c>
     </row>
@@ -15027,15 +14923,14 @@
       <c r="H130" s="2">
         <v>6.4401000000000002</v>
       </c>
-      <c r="I130" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DEPAY</v>
+      <c r="I130" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K130" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.80829065655525312</v>
       </c>
     </row>
@@ -15064,15 +14959,14 @@
       <c r="H131" s="2">
         <v>5.3535000000000004</v>
       </c>
-      <c r="I131" s="1" t="str">
-        <f t="shared" ref="I131:I133" si="4">IF(F131&lt;40,"ESTEVÃO","DEPAY")</f>
-        <v>DEPAY</v>
+      <c r="I131" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K131" s="1">
-        <f t="shared" ref="K131:K133" si="5">(H131-$H$136)/$H$137</f>
+        <f t="shared" ref="K131:K133" si="2">(H131-$H$136)/$H$137</f>
         <v>-0.17900262908720221</v>
       </c>
     </row>
@@ -15101,15 +14995,14 @@
       <c r="H132" s="2">
         <v>3.7593999999999999</v>
       </c>
-      <c r="I132" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>DEPAY</v>
+      <c r="I132" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K132" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-1.6274143966581933</v>
       </c>
     </row>
@@ -15138,39 +15031,37 @@
       <c r="H133" s="2">
         <v>3.2991999999999999</v>
       </c>
-      <c r="I133" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>DEPAY</v>
+      <c r="I133" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K133" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-2.0455557274631428</v>
       </c>
       <c r="M133" s="1" t="str">
         <f>J133</f>
         <v>BAIXA</v>
       </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I134" s="7"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H136" s="5">
         <f>AVERAGE(H1:H133)</f>
         <v>5.5505075757575781</v>
       </c>
-      <c r="I136" s="1" t="s">
-        <v>272</v>
-      </c>
+      <c r="I136" s="5"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H137" s="5">
         <f>_xlfn.STDEV.S(H1:H133)</f>
         <v>1.1005848168945291</v>
       </c>
-      <c r="I137" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="I137" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D133">

</xml_diff>